<commit_message>
Fix Aarons 5x5x5 times (entered as 3x3x3)
</commit_message>
<xml_diff>
--- a/data/2021-01-19/SCW Weekly Comp 2021-01-19 (Responses).xlsx
+++ b/data/2021-01-19/SCW Weekly Comp 2021-01-19 (Responses).xlsx
@@ -1,14 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2021-01-19\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C049A85C-A8E6-46AA-97BA-89EA82183519}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$CY$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$CY$74</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -810,23 +820,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -834,43 +847,46 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1060,26 +1076,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:CY74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="109" width="21.57"/>
+    <col min="1" max="109" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1390,9 +1409,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44216.15591497685</v>
+        <v>44216.155914976851</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -1431,9 +1450,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44216.43762635416</v>
+        <v>44216.437626354164</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>27</v>
@@ -1466,9 +1485,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44216.52950851852</v>
+        <v>44216.529508518521</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
@@ -1498,9 +1517,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44216.61284872685</v>
+        <v>44216.612848726851</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
@@ -1539,7 +1558,7 @@
         <v>38.29</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44216.6637996875</v>
       </c>
@@ -1583,9 +1602,9 @@
         <v>44.02</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44216.70939726852</v>
+        <v>44216.709397268518</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>46</v>
@@ -1618,9 +1637,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44216.72848579861</v>
+        <v>44216.728485798609</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>46</v>
@@ -1653,9 +1672,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44216.87035831019</v>
+        <v>44216.870358310189</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>59</v>
@@ -1670,10 +1689,10 @@
         <v>61</v>
       </c>
       <c r="CJ9" s="3">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44216.871393113426</v>
       </c>
@@ -1708,9 +1727,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44216.88681108796</v>
+        <v>44216.886811087963</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -1734,7 +1753,7 @@
         <v>33.11</v>
       </c>
       <c r="J11" s="3">
-        <v>36.12</v>
+        <v>36.119999999999997</v>
       </c>
       <c r="K11" s="3">
         <v>33.06</v>
@@ -1749,9 +1768,9 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44217.36156549769</v>
+        <v>44217.361565497689</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>27</v>
@@ -1784,9 +1803,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44217.42078918981</v>
+        <v>44217.420789189811</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>73</v>
@@ -1816,7 +1835,7 @@
         <v>29.65</v>
       </c>
       <c r="S13" s="3">
-        <v>32.77</v>
+        <v>32.770000000000003</v>
       </c>
       <c r="T13" s="3">
         <v>22.55</v>
@@ -1825,9 +1844,9 @@
         <v>26.21</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44217.6228820949</v>
+        <v>44217.622882094904</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>17</v>
@@ -1860,9 +1879,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>44217.70332665509</v>
+        <v>44217.703326655093</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -1880,7 +1899,7 @@
         <v>80</v>
       </c>
       <c r="O15" s="3">
-        <v>37.02</v>
+        <v>37.020000000000003</v>
       </c>
       <c r="P15" s="3">
         <v>31.4</v>
@@ -1892,7 +1911,7 @@
         <v>52.55</v>
       </c>
       <c r="S15" s="3">
-        <v>34.91</v>
+        <v>34.909999999999997</v>
       </c>
       <c r="T15" s="3">
         <v>31.4</v>
@@ -1901,9 +1920,9 @@
         <v>35.86</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44217.71599831019</v>
+        <v>44217.715998310188</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
@@ -1942,9 +1961,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44217.96978896991</v>
+        <v>44217.969788969909</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>46</v>
@@ -1983,7 +2002,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44218.374185775465</v>
       </c>
@@ -2024,9 +2043,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44218.51495121528</v>
+        <v>44218.514951215278</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>99</v>
@@ -2065,7 +2084,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44218.539671527775</v>
       </c>
@@ -2097,7 +2116,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44218.63971625</v>
       </c>
@@ -2135,9 +2154,9 @@
         <v>22.71</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44218.68003553241</v>
+        <v>44218.680035532409</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>27</v>
@@ -2176,7 +2195,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44218.839302719905</v>
       </c>
@@ -2217,9 +2236,9 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>44219.17993789352</v>
+        <v>44219.179937893517</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>73</v>
@@ -2255,12 +2274,12 @@
         <v>33.83</v>
       </c>
       <c r="AZ24" s="3">
-        <v>40.63</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>40.630000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44219.57078275463</v>
+        <v>44219.570782754628</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>46</v>
@@ -2281,13 +2300,13 @@
         <v>17.47</v>
       </c>
       <c r="P25" s="3">
-        <v>18.33</v>
+        <v>18.329999999999998</v>
       </c>
       <c r="Q25" s="3">
         <v>17.39</v>
       </c>
       <c r="R25" s="3">
-        <v>19.44</v>
+        <v>19.440000000000001</v>
       </c>
       <c r="S25" s="3">
         <v>18.03</v>
@@ -2296,10 +2315,10 @@
         <v>17.39</v>
       </c>
       <c r="U25" s="3">
-        <v>17.94</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44219.776819039354</v>
       </c>
@@ -2328,10 +2347,10 @@
         <v>15.71</v>
       </c>
       <c r="CF26" s="3">
-        <v>16.83</v>
+        <v>16.829999999999998</v>
       </c>
       <c r="CG26" s="3">
-        <v>18.81</v>
+        <v>18.809999999999999</v>
       </c>
       <c r="CH26" s="3">
         <v>15.14</v>
@@ -2340,9 +2359,9 @@
         <v>16.04</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44219.78003513889</v>
+        <v>44219.780035138887</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
@@ -2378,9 +2397,9 @@
         <v>16.36</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44219.78088384259</v>
+        <v>44219.780883842592</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>36</v>
@@ -2416,7 +2435,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44219.96359954861</v>
       </c>
@@ -2445,7 +2464,7 @@
         <v>21.33</v>
       </c>
       <c r="Q29" s="3">
-        <v>16.67</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="R29" s="3">
         <v>18.07</v>
@@ -2454,13 +2473,13 @@
         <v>20.23</v>
       </c>
       <c r="T29" s="3">
-        <v>16.67</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="U29" s="3">
         <v>19.88</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44219.96776944444</v>
       </c>
@@ -2492,16 +2511,16 @@
         <v>8.24</v>
       </c>
       <c r="L30" s="3">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="M30" s="3">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="N30" s="3">
         <v>6.98</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44219.99797538195</v>
       </c>
@@ -2536,9 +2555,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44220.01283072917</v>
+        <v>44220.012830729167</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>136</v>
@@ -2577,7 +2596,7 @@
         <v>17.07</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44220.510188333334</v>
       </c>
@@ -2615,10 +2634,10 @@
         <v>19.3</v>
       </c>
       <c r="U33" s="3">
-        <v>20.26</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>20.260000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44220.514196840275</v>
       </c>
@@ -2653,7 +2672,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44220.575359016206</v>
       </c>
@@ -2667,7 +2686,7 @@
         <v>100</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>151</v>
@@ -2675,31 +2694,31 @@
       <c r="G35" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="O35" s="3" t="s">
+      <c r="AC35" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="P35" s="3" t="s">
+      <c r="AD35" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q35" s="3" t="s">
+      <c r="AE35" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="R35" s="3" t="s">
+      <c r="AF35" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="S35" s="3" t="s">
+      <c r="AG35" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="T35" s="3" t="s">
+      <c r="AH35" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="U35" s="3" t="s">
+      <c r="AI35" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>44220.61770094908</v>
+        <v>44220.617700949078</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>46</v>
@@ -2726,7 +2745,7 @@
         <v>29.28</v>
       </c>
       <c r="AW36" s="3">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="AX36" s="3">
         <v>34.69</v>
@@ -2738,9 +2757,9 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44220.62230246528</v>
+        <v>44220.622302465279</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>27</v>
@@ -2779,7 +2798,7 @@
         <v>19.25</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44220.815666574075</v>
       </c>
@@ -2799,10 +2818,10 @@
         <v>161</v>
       </c>
       <c r="O38" s="3">
-        <v>32.13</v>
+        <v>32.130000000000003</v>
       </c>
       <c r="P38" s="3">
-        <v>34.62</v>
+        <v>34.619999999999997</v>
       </c>
       <c r="Q38" s="3">
         <v>28.99</v>
@@ -2820,9 +2839,9 @@
         <v>31.74</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44220.8185525463</v>
+        <v>44220.818552546298</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>126</v>
@@ -2849,7 +2868,7 @@
         <v>7.89</v>
       </c>
       <c r="J39" s="3">
-        <v>8.45</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="K39" s="3">
         <v>6.99</v>
@@ -2864,9 +2883,9 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44220.81990298611</v>
+        <v>44220.819902986113</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>126</v>
@@ -2896,7 +2915,7 @@
         <v>10.7</v>
       </c>
       <c r="BL40" s="3">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="BM40" s="3">
         <v>10.7</v>
@@ -2905,9 +2924,9 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44220.8656899537</v>
+        <v>44220.865689953702</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>166</v>
@@ -2943,9 +2962,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44220.9052897338</v>
+        <v>44220.905289733797</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>171</v>
@@ -2984,9 +3003,9 @@
         <v>29.35</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44220.93311215278</v>
+        <v>44220.933112152779</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>171</v>
@@ -3025,9 +3044,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>44220.95348804398</v>
+        <v>44220.953488043982</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>179</v>
@@ -3048,9 +3067,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44221.10548746528</v>
+        <v>44221.105487465276</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>182</v>
@@ -3089,9 +3108,9 @@
         <v>12.36</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44221.11267796296</v>
+        <v>44221.112677962963</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>182</v>
@@ -3112,7 +3131,7 @@
         <v>31.05</v>
       </c>
       <c r="P46" s="3">
-        <v>36.52</v>
+        <v>36.520000000000003</v>
       </c>
       <c r="Q46" s="3">
         <v>48.31</v>
@@ -3121,7 +3140,7 @@
         <v>31.13</v>
       </c>
       <c r="S46" s="3">
-        <v>36.91</v>
+        <v>36.909999999999997</v>
       </c>
       <c r="T46" s="3">
         <v>31.05</v>
@@ -3130,9 +3149,9 @@
         <v>34.85</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44221.11616621527</v>
+        <v>44221.116166215274</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>182</v>
@@ -3171,9 +3190,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:93" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44221.11934796296</v>
+        <v>44221.119347962958</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>182</v>
@@ -3215,9 +3234,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44221.12206306713</v>
+        <v>44221.122063067131</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>182</v>
@@ -3256,9 +3275,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>44221.21439221065</v>
+        <v>44221.214392210648</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>201</v>
@@ -3279,7 +3298,7 @@
         <v>26.51</v>
       </c>
       <c r="BW50" s="3">
-        <v>33.88</v>
+        <v>33.880000000000003</v>
       </c>
       <c r="BX50" s="3">
         <v>19.07</v>
@@ -3297,9 +3316,9 @@
         <v>30.16</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>44221.21509157408</v>
+        <v>44221.215091574079</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>201</v>
@@ -3329,7 +3348,7 @@
         <v>10.84</v>
       </c>
       <c r="BL51" s="3">
-        <v>18.26</v>
+        <v>18.260000000000002</v>
       </c>
       <c r="BM51" s="3">
         <v>10.78</v>
@@ -3338,7 +3357,7 @@
         <v>11.72</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44221.21583685185</v>
       </c>
@@ -3367,21 +3386,21 @@
         <v>9.98</v>
       </c>
       <c r="K52" s="3">
-        <v>9.38</v>
+        <v>9.3800000000000008</v>
       </c>
       <c r="L52" s="3">
         <v>10.9</v>
       </c>
       <c r="M52" s="3">
-        <v>9.38</v>
+        <v>9.3800000000000008</v>
       </c>
       <c r="N52" s="3">
         <v>10.26</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>44221.21662986111</v>
+        <v>44221.216629861112</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>201</v>
@@ -3420,9 +3439,9 @@
         <v>24.56</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>44221.21761287037</v>
+        <v>44221.217612870372</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>201</v>
@@ -3461,9 +3480,9 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>44221.39319311343</v>
+        <v>44221.393193113428</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>144</v>
@@ -3502,9 +3521,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>44221.41914525463</v>
+        <v>44221.419145254629</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>144</v>
@@ -3543,7 +3562,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44221.421166712964</v>
       </c>
@@ -3563,7 +3582,7 @@
         <v>226</v>
       </c>
       <c r="O57" s="3">
-        <v>19.42</v>
+        <v>19.420000000000002</v>
       </c>
       <c r="P57" s="3">
         <v>18.18</v>
@@ -3584,9 +3603,9 @@
         <v>17.97</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>44221.42191113426</v>
+        <v>44221.421911134261</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>224</v>
@@ -3607,7 +3626,7 @@
         <v>37.07</v>
       </c>
       <c r="AU58" s="3">
-        <v>33.84</v>
+        <v>33.840000000000003</v>
       </c>
       <c r="AV58" s="3">
         <v>28.4</v>
@@ -3622,12 +3641,12 @@
         <v>28.4</v>
       </c>
       <c r="AZ58" s="3">
-        <v>35.62</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>35.619999999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>44221.52604890046</v>
+        <v>44221.526048900458</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>46</v>
@@ -3666,7 +3685,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44221.606823298614</v>
       </c>
@@ -3683,12 +3702,12 @@
         <v>235</v>
       </c>
       <c r="CJ60" s="3">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>44221.60783738426</v>
+        <v>44221.607837384261</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>36</v>
@@ -3718,7 +3737,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44221.609470613424</v>
       </c>
@@ -3753,9 +3772,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>44221.79113370371</v>
+        <v>44221.791133703708</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>239</v>
@@ -3776,7 +3795,7 @@
         <v>7.54</v>
       </c>
       <c r="BI63" s="3">
-        <v>8.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="BJ63" s="3">
         <v>6.41</v>
@@ -3794,7 +3813,7 @@
         <v>7.38</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44221.791864259256</v>
       </c>
@@ -3835,7 +3854,7 @@
         <v>6.78</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44221.792611365745</v>
       </c>
@@ -3876,9 +3895,9 @@
         <v>30.95</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>44221.79318482639</v>
+        <v>44221.793184826391</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>239</v>
@@ -3917,9 +3936,9 @@
         <v>13.22</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>44221.81165081018</v>
+        <v>44221.811650810181</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>239</v>
@@ -3955,12 +3974,12 @@
         <v>13.55</v>
       </c>
       <c r="U67" s="3">
-        <v>16.24</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>16.239999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>44221.81223927083</v>
+        <v>44221.812239270832</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>239</v>
@@ -3999,9 +4018,9 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>44221.81287310185</v>
+        <v>44221.812873101851</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>239</v>
@@ -4040,7 +4059,7 @@
         <v>27.32</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44221.81353561343</v>
       </c>
@@ -4081,9 +4100,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>44221.82050369213</v>
+        <v>44221.820503692128</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>239</v>
@@ -4122,9 +4141,9 @@
         <v>58.26</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>44221.82116961805</v>
+        <v>44221.821169618051</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>239</v>
@@ -4163,7 +4182,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44221.821694756945</v>
       </c>
@@ -4198,9 +4217,9 @@
         <v>259</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>44221.82216200231</v>
+        <v>44221.822162002311</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>239</v>
@@ -4234,82 +4253,82 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$CY$74"/>
+  <autoFilter ref="A1:CY74" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
-    <hyperlink r:id="rId3" ref="F4"/>
-    <hyperlink r:id="rId4" ref="F5"/>
-    <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" ref="F7"/>
-    <hyperlink r:id="rId7" ref="F8"/>
-    <hyperlink r:id="rId8" ref="F9"/>
-    <hyperlink r:id="rId9" ref="F10"/>
-    <hyperlink r:id="rId10" ref="F11"/>
-    <hyperlink r:id="rId11" ref="F12"/>
-    <hyperlink r:id="rId12" ref="F13"/>
-    <hyperlink r:id="rId13" ref="F14"/>
-    <hyperlink r:id="rId14" ref="F15"/>
-    <hyperlink r:id="rId15" ref="F16"/>
-    <hyperlink r:id="rId16" ref="F17"/>
-    <hyperlink r:id="rId17" ref="F18"/>
-    <hyperlink r:id="rId18" ref="F19"/>
-    <hyperlink r:id="rId19" ref="F20"/>
-    <hyperlink r:id="rId20" ref="F21"/>
-    <hyperlink r:id="rId21" ref="F22"/>
-    <hyperlink r:id="rId22" ref="F23"/>
-    <hyperlink r:id="rId23" ref="F24"/>
-    <hyperlink r:id="rId24" ref="F25"/>
-    <hyperlink r:id="rId25" ref="F26"/>
-    <hyperlink r:id="rId26" ref="F27"/>
-    <hyperlink r:id="rId27" ref="F28"/>
-    <hyperlink r:id="rId28" ref="F29"/>
-    <hyperlink r:id="rId29" ref="F30"/>
-    <hyperlink r:id="rId30" ref="F31"/>
-    <hyperlink r:id="rId31" ref="F32"/>
-    <hyperlink r:id="rId32" ref="F33"/>
-    <hyperlink r:id="rId33" ref="F34"/>
-    <hyperlink r:id="rId34" ref="F35"/>
-    <hyperlink r:id="rId35" ref="F36"/>
-    <hyperlink r:id="rId36" ref="F37"/>
-    <hyperlink r:id="rId37" ref="F38"/>
-    <hyperlink r:id="rId38" ref="F39"/>
-    <hyperlink r:id="rId39" ref="F40"/>
-    <hyperlink r:id="rId40" ref="F41"/>
-    <hyperlink r:id="rId41" ref="F42"/>
-    <hyperlink r:id="rId42" ref="F43"/>
-    <hyperlink r:id="rId43" ref="F44"/>
-    <hyperlink r:id="rId44" ref="F45"/>
-    <hyperlink r:id="rId45" ref="F46"/>
-    <hyperlink r:id="rId46" ref="F47"/>
-    <hyperlink r:id="rId47" ref="F48"/>
-    <hyperlink r:id="rId48" ref="F49"/>
-    <hyperlink r:id="rId49" ref="F50"/>
-    <hyperlink r:id="rId50" ref="F51"/>
-    <hyperlink r:id="rId51" ref="F52"/>
-    <hyperlink r:id="rId52" ref="F53"/>
-    <hyperlink r:id="rId53" ref="F54"/>
-    <hyperlink r:id="rId54" ref="F55"/>
-    <hyperlink r:id="rId55" ref="F56"/>
-    <hyperlink r:id="rId56" ref="F57"/>
-    <hyperlink r:id="rId57" ref="F58"/>
-    <hyperlink r:id="rId58" ref="F59"/>
-    <hyperlink r:id="rId59" ref="F60"/>
-    <hyperlink r:id="rId60" ref="F61"/>
-    <hyperlink r:id="rId61" ref="F62"/>
-    <hyperlink r:id="rId62" ref="F63"/>
-    <hyperlink r:id="rId63" ref="F64"/>
-    <hyperlink r:id="rId64" ref="F65"/>
-    <hyperlink r:id="rId65" ref="F66"/>
-    <hyperlink r:id="rId66" ref="F67"/>
-    <hyperlink r:id="rId67" ref="F68"/>
-    <hyperlink r:id="rId68" ref="F69"/>
-    <hyperlink r:id="rId69" ref="F70"/>
-    <hyperlink r:id="rId70" ref="F71"/>
-    <hyperlink r:id="rId71" ref="F72"/>
-    <hyperlink r:id="rId72" ref="F73"/>
-    <hyperlink r:id="rId73" ref="F74"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="F74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
   </hyperlinks>
-  <drawing r:id="rId74"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>